<commit_message>
add import lop from excel
</commit_message>
<xml_diff>
--- a/database/data_lop.xlsx
+++ b/database/data_lop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DangKyHocPhan\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9EDA39-CC1A-41C8-9F7A-D30CF0FCDE7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4FDF5A-4F1D-46A1-BD05-008B6C9B5B31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9684" xr2:uid="{4C14E746-97DD-45DA-B484-C5D455A71618}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>malop</t>
   </si>
@@ -37,6 +37,57 @@
   </si>
   <si>
     <t>makhoa</t>
+  </si>
+  <si>
+    <t>DHCN3A</t>
+  </si>
+  <si>
+    <t>Đại học công nghệ 3A</t>
+  </si>
+  <si>
+    <t>CNTT-TCKGM</t>
+  </si>
+  <si>
+    <t>2016-2020</t>
+  </si>
+  <si>
+    <t>DHCN3B</t>
+  </si>
+  <si>
+    <t>Đại học công nghệ 3B</t>
+  </si>
+  <si>
+    <t>DHCN4</t>
+  </si>
+  <si>
+    <t>Đại học công nghệ 4</t>
+  </si>
+  <si>
+    <t>2017-2021</t>
+  </si>
+  <si>
+    <t>DHCN5</t>
+  </si>
+  <si>
+    <t>Đại học công nghệ 5</t>
+  </si>
+  <si>
+    <t>2018-2022</t>
+  </si>
+  <si>
+    <t>DTVT3</t>
+  </si>
+  <si>
+    <t>Điện tử viễn thông 3</t>
+  </si>
+  <si>
+    <t>DTVT</t>
+  </si>
+  <si>
+    <t>DTVT4</t>
+  </si>
+  <si>
+    <t>Điện tử viễn thông 4</t>
   </si>
 </sst>
 </file>
@@ -80,9 +131,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,29 +451,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B91853-1060-4725-B73E-404FBD4765E4}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="10.59765625" style="1"/>
+    <col min="1" max="1" width="13.796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.09765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.19921875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.59765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>